<commit_message>
Updated ITA model - 2025-08-10 01:53
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_and_Hydro.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_and_Hydro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6EF95F3-C934-4B69-84A5-99455BE7E9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B417C47-3A17-4F35-BA68-522B7CCF6F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -652,24 +652,24 @@
     <t>solar resource -- CF class spv-ITA_13 -- cost class 1</t>
   </si>
   <si>
+    <t>e_spv-ITA_13_c4</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-ITA_13 -- cost class 4</t>
+  </si>
+  <si>
+    <t>e_spv-ITA_13_c3</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-ITA_13 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_spv-ITA_13_c2</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-ITA_13 -- cost class 2</t>
   </si>
   <si>
-    <t>e_spv-ITA_13_c4</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-ITA_13 -- cost class 4</t>
-  </si>
-  <si>
-    <t>e_spv-ITA_13_c3</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-ITA_13 -- cost class 3</t>
-  </si>
-  <si>
     <t>comm-out</t>
   </si>
   <si>
@@ -706,18 +706,18 @@
     <t>wind resource -- CF class won-ITA_33 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_32_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_32 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-ITA_32_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_32 -- cost class 1</t>
   </si>
   <si>
-    <t>e_won-ITA_32_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_32 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_won-ITA_32_c2</t>
   </si>
   <si>
@@ -748,22 +748,22 @@
     <t>wind resource -- CF class won-ITA_29 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_29_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_29 -- cost class 3</t>
+  </si>
+  <si>
+    <t>e_won-ITA_29_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-ITA_29_c5</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_29 -- cost class 5</t>
-  </si>
-  <si>
-    <t>e_won-ITA_29_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_29 -- cost class 3</t>
-  </si>
-  <si>
-    <t>e_won-ITA_29_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
   </si>
   <si>
     <t>e_won-ITA_28_c1</t>
@@ -4089,7 +4089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B0AE9F-91B5-4D03-B303-9B2A18FF572F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B18449-317A-422E-9D27-793BB73FF8F1}">
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5278,7 +5278,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P30" s="32">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:16">
@@ -5319,7 +5319,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P31" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -5360,7 +5360,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P32" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5372,7 +5372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB659A9-0FDE-40E7-9070-2F2E2118ED25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CFFBE4-9193-45A7-996D-122CF653FAC4}">
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5607,16 +5607,16 @@
         <v>386</v>
       </c>
       <c r="M7" s="33">
-        <v>1.5E-3</v>
+        <v>2.4990000000000001</v>
       </c>
       <c r="N7" s="36">
         <v>0.32200000000000001</v>
       </c>
       <c r="O7" s="37">
-        <v>31.372355844942916</v>
+        <v>39.630069093581724</v>
       </c>
       <c r="P7" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -5648,16 +5648,16 @@
         <v>386</v>
       </c>
       <c r="M8" s="32">
-        <v>2.4990000000000001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="N8" s="34">
         <v>0.32200000000000001</v>
       </c>
       <c r="O8" s="35">
-        <v>39.630069093581724</v>
+        <v>31.372355844942916</v>
       </c>
       <c r="P8" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -5903,7 +5903,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P14" s="32">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -5944,7 +5944,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P15" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -5985,7 +5985,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P16" s="32">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:16">

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-10 20:31
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_and_Hydro.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_and_Hydro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B417C47-3A17-4F35-BA68-522B7CCF6F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E16F535F-DAA3-49C9-A792-74C51C622E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -652,18 +652,18 @@
     <t>solar resource -- CF class spv-ITA_13 -- cost class 1</t>
   </si>
   <si>
+    <t>e_spv-ITA_13_c3</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-ITA_13 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_spv-ITA_13_c4</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-ITA_13 -- cost class 4</t>
   </si>
   <si>
-    <t>e_spv-ITA_13_c3</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-ITA_13 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_spv-ITA_13_c2</t>
   </si>
   <si>
@@ -706,18 +706,18 @@
     <t>wind resource -- CF class won-ITA_33 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_32_c1</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_32 -- cost class 1</t>
+  </si>
+  <si>
     <t>e_won-ITA_32_c3</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_32 -- cost class 3</t>
   </si>
   <si>
-    <t>e_won-ITA_32_c1</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_32 -- cost class 1</t>
-  </si>
-  <si>
     <t>e_won-ITA_32_c2</t>
   </si>
   <si>
@@ -748,24 +748,24 @@
     <t>wind resource -- CF class won-ITA_29 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_29_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
+  </si>
+  <si>
+    <t>e_won-ITA_29_c5</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_29 -- cost class 5</t>
+  </si>
+  <si>
     <t>e_won-ITA_29_c3</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_29 -- cost class 3</t>
   </si>
   <si>
-    <t>e_won-ITA_29_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
-  </si>
-  <si>
-    <t>e_won-ITA_29_c5</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_29 -- cost class 5</t>
-  </si>
-  <si>
     <t>e_won-ITA_28_c1</t>
   </si>
   <si>
@@ -808,18 +808,18 @@
     <t>wind resource -- CF class won-ITA_26 -- cost class 2</t>
   </si>
   <si>
+    <t>e_won-ITA_25_c1</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_25 -- cost class 1</t>
+  </si>
+  <si>
     <t>e_won-ITA_25_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
   </si>
   <si>
-    <t>e_won-ITA_25_c1</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_25 -- cost class 1</t>
-  </si>
-  <si>
     <t>e_won-ITA_25_c3</t>
   </si>
   <si>
@@ -1252,16 +1252,16 @@
     <t>wind resource -- CF class won-ITA_11 -- cost class 3</t>
   </si>
   <si>
+    <t>e_won-ITA_10_c1</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_10 -- cost class 1</t>
+  </si>
+  <si>
     <t>e_won-ITA_10_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_10 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-ITA_10_c1</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_10 -- cost class 1</t>
   </si>
   <si>
     <t>elc_won-ITA</t>
@@ -4089,7 +4089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B18449-317A-422E-9D27-793BB73FF8F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DD94D2-5BBF-47CE-954B-DD320D9048DF}">
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5278,7 +5278,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P30" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:16">
@@ -5319,7 +5319,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P31" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -5372,7 +5372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CFFBE4-9193-45A7-996D-122CF653FAC4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC67C071-4326-42D3-9E85-04939247AD24}">
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5607,16 +5607,16 @@
         <v>386</v>
       </c>
       <c r="M7" s="33">
-        <v>2.4990000000000001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="N7" s="36">
         <v>0.32200000000000001</v>
       </c>
       <c r="O7" s="37">
-        <v>39.630069093581724</v>
+        <v>31.372355844942916</v>
       </c>
       <c r="P7" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -5648,16 +5648,16 @@
         <v>386</v>
       </c>
       <c r="M8" s="32">
-        <v>1.5E-3</v>
+        <v>2.4990000000000001</v>
       </c>
       <c r="N8" s="34">
         <v>0.32200000000000001</v>
       </c>
       <c r="O8" s="35">
-        <v>31.372355844942916</v>
+        <v>39.630069093581724</v>
       </c>
       <c r="P8" s="32">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -5903,7 +5903,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P14" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -5944,7 +5944,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P15" s="33">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -5985,7 +5985,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P16" s="32">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -6313,7 +6313,7 @@
         <v>39.368264706413946</v>
       </c>
       <c r="P24" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -6354,7 +6354,7 @@
         <v>39.368264706413946</v>
       </c>
       <c r="P25" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -9347,7 +9347,7 @@
         <v>74.16840218346799</v>
       </c>
       <c r="P98" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:16">
@@ -9388,7 +9388,7 @@
         <v>74.16840218346799</v>
       </c>
       <c r="P99" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-10 22:40
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_and_Hydro.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_and_Hydro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E16F535F-DAA3-49C9-A792-74C51C622E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E235B47F-DC78-48B1-97EE-07274E4C38FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -652,18 +652,18 @@
     <t>solar resource -- CF class spv-ITA_13 -- cost class 1</t>
   </si>
   <si>
+    <t>e_spv-ITA_13_c4</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-ITA_13 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_spv-ITA_13_c3</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-ITA_13 -- cost class 3</t>
   </si>
   <si>
-    <t>e_spv-ITA_13_c4</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-ITA_13 -- cost class 4</t>
-  </si>
-  <si>
     <t>e_spv-ITA_13_c2</t>
   </si>
   <si>
@@ -706,18 +706,18 @@
     <t>wind resource -- CF class won-ITA_33 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_32_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_32 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-ITA_32_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_32 -- cost class 1</t>
   </si>
   <si>
-    <t>e_won-ITA_32_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_32 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_won-ITA_32_c2</t>
   </si>
   <si>
@@ -748,24 +748,24 @@
     <t>wind resource -- CF class won-ITA_29 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_29_c5</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_29 -- cost class 5</t>
+  </si>
+  <si>
+    <t>e_won-ITA_29_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_29 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-ITA_29_c4</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
   </si>
   <si>
-    <t>e_won-ITA_29_c5</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_29 -- cost class 5</t>
-  </si>
-  <si>
-    <t>e_won-ITA_29_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_29 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_won-ITA_28_c1</t>
   </si>
   <si>
@@ -820,18 +820,18 @@
     <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
   </si>
   <si>
+    <t>e_won-ITA_25_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_25 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-ITA_25_c3</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_25 -- cost class 3</t>
   </si>
   <si>
-    <t>e_won-ITA_25_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_25 -- cost class 4</t>
-  </si>
-  <si>
     <t>e_won-ITA_24_c2</t>
   </si>
   <si>
@@ -1228,18 +1228,18 @@
     <t>wind resource -- CF class won-ITA_11 -- cost class 4</t>
   </si>
   <si>
+    <t>e_won-ITA_11_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_11 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-ITA_11_c5</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_11 -- cost class 5</t>
   </si>
   <si>
-    <t>e_won-ITA_11_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_11 -- cost class 2</t>
-  </si>
-  <si>
     <t>e_won-ITA_11_c1</t>
   </si>
   <si>
@@ -1252,16 +1252,16 @@
     <t>wind resource -- CF class won-ITA_11 -- cost class 3</t>
   </si>
   <si>
+    <t>e_won-ITA_10_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_10 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-ITA_10_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_10 -- cost class 1</t>
-  </si>
-  <si>
-    <t>e_won-ITA_10_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_10 -- cost class 2</t>
   </si>
   <si>
     <t>elc_won-ITA</t>
@@ -4089,7 +4089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DD94D2-5BBF-47CE-954B-DD320D9048DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B4FC8B-334C-490B-9163-439BD382D868}">
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5278,7 +5278,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P30" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:16">
@@ -5319,7 +5319,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P31" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -5372,7 +5372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC67C071-4326-42D3-9E85-04939247AD24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0412ADD0-2A68-4C25-876D-A10CA9B7C18B}">
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5607,16 +5607,16 @@
         <v>386</v>
       </c>
       <c r="M7" s="33">
-        <v>1.5E-3</v>
+        <v>2.4990000000000001</v>
       </c>
       <c r="N7" s="36">
         <v>0.32200000000000001</v>
       </c>
       <c r="O7" s="37">
-        <v>31.372355844942916</v>
+        <v>39.630069093581724</v>
       </c>
       <c r="P7" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -5648,16 +5648,16 @@
         <v>386</v>
       </c>
       <c r="M8" s="32">
-        <v>2.4990000000000001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="N8" s="34">
         <v>0.32200000000000001</v>
       </c>
       <c r="O8" s="35">
-        <v>39.630069093581724</v>
+        <v>31.372355844942916</v>
       </c>
       <c r="P8" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -5903,7 +5903,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P14" s="32">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -5944,7 +5944,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P15" s="33">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -5985,7 +5985,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P16" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -6386,16 +6386,16 @@
         <v>386</v>
       </c>
       <c r="M26" s="32">
-        <v>3.2032500000000002</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="N26" s="34">
         <v>0.245</v>
       </c>
       <c r="O26" s="35">
-        <v>42.969340484621256</v>
+        <v>107.03467623779731</v>
       </c>
       <c r="P26" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -6427,16 +6427,16 @@
         <v>386</v>
       </c>
       <c r="M27" s="33">
-        <v>4.4999999999999997E-3</v>
+        <v>3.2032500000000002</v>
       </c>
       <c r="N27" s="36">
         <v>0.245</v>
       </c>
       <c r="O27" s="37">
-        <v>107.03467623779731</v>
+        <v>42.969340484621256</v>
       </c>
       <c r="P27" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:16">
@@ -9174,16 +9174,16 @@
         <v>386</v>
       </c>
       <c r="M94" s="32">
-        <v>0.43575000000000003</v>
+        <v>0.03</v>
       </c>
       <c r="N94" s="34">
         <v>0.113</v>
       </c>
       <c r="O94" s="35">
-        <v>120.30091898433189</v>
+        <v>94.983314628615091</v>
       </c>
       <c r="P94" s="32">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="2:16">
@@ -9215,16 +9215,16 @@
         <v>386</v>
       </c>
       <c r="M95" s="33">
-        <v>0.03</v>
+        <v>0.43575000000000003</v>
       </c>
       <c r="N95" s="36">
         <v>0.113</v>
       </c>
       <c r="O95" s="37">
-        <v>94.983314628615091</v>
+        <v>120.30091898433189</v>
       </c>
       <c r="P95" s="33">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="2:16">
@@ -9347,7 +9347,7 @@
         <v>74.16840218346799</v>
       </c>
       <c r="P98" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="2:16">
@@ -9388,7 +9388,7 @@
         <v>74.16840218346799</v>
       </c>
       <c r="P99" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>